<commit_message>
fix template rows mis-index
</commit_message>
<xml_diff>
--- a/testdata/out_validation_tmpl.xlsx
+++ b/testdata/out_validation_tmpl.xlsx
@@ -1,62 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <ma:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <ma:fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10307"/>
-  <ma:workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <ma:fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <ma:workbookPr/>
   <ma:bookViews>
-    <ma:workbookView xWindow="5000" yWindow="3960" windowWidth="25520" windowHeight="16000" tabRatio="500"/>
+    <ma:workbookView windowHeight="17980" tabRatio="500"/>
   </ma:bookViews>
   <ma:sheets>
     <ma:sheet name="会员" sheetId="1" r:id="rId1"/>
     <ma:sheet name="Validation" sheetId="4" r:id="rId2"/>
   </ma:sheets>
   <ma:definedNames>
-    <ma:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">会员!$A$1:$A$2</ma:definedName>
+    <ma:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">会员!$C$2:$C$3</ma:definedName>
   </ma:definedNames>
-  <ma:calcPr calcId="140000"/>
-  <ma:extLst>
-    <ma:ext uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <m:workbookPr xmlns:m="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultImageDpi="32767"/>
-    </ma:ext>
-    <ma:ext uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <m:ArchID xmlns:m="http://schemas.microsoft.com/office/mac/excel/2008/main" Flags="2"/>
-    </ma:ext>
-  </ma:extLst>
+  <ma:calcPr calcId="144525"/>
 </ma:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="11" uniqueCount="11">
+<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="10" uniqueCount="10">
   <ma:si>
     <ma:t>会员总数</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
+  </ma:si>
+  <ma:si>
+    <ma:t>区域</ma:t>
   </ma:si>
   <ma:si>
     <ma:t>其中：新增</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
   </ma:si>
   <ma:si>
     <ma:t>其中：有效</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
-  </ma:si>
-  <ma:si>
-    <ma:t>区域</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
   </ma:si>
   <ma:si>
     <ma:t>A</ma:t>
   </ma:si>
   <ma:si>
-    <ma:t>A</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
-  </ma:si>
-  <ma:si>
     <ma:t>B</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
   </ma:si>
   <ma:si>
     <ma:t>C</ma:t>
-    <ma:phoneticPr fontId="1" type="noConversion"/>
   </ma:si>
   <ma:si>
     <ma:t>A</ma:t>
@@ -72,55 +54,177 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <ma:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <ma:fonts count="6">
+  <ma:numFmts count="4">
+    <ma:numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <ma:numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <ma:numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <ma:numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </ma:numFmts>
+  <ma:fonts count="22">
     <ma:font>
       <ma:name val="宋体"/>
       <ma:charset val="134"/>
-      <ma:family val="2"/>
       <ma:color theme="1"/>
       <ma:sz val="12"/>
       <ma:scheme val="minor"/>
     </ma:font>
     <ma:font>
-      <ma:name val="宋体"/>
-      <ma:charset val="134"/>
-      <ma:family val="2"/>
-      <ma:sz val="9"/>
-      <ma:scheme val="minor"/>
-    </ma:font>
-    <ma:font>
       <ma:name val="Hiragino Sans GB W3"/>
       <ma:charset val="134"/>
-      <ma:family val="3"/>
       <ma:color theme="1"/>
       <ma:sz val="14"/>
     </ma:font>
     <ma:font>
-      <ma:name val="宋体"/>
-      <ma:charset val="134"/>
-      <ma:family val="2"/>
-      <ma:color theme="10"/>
-      <ma:sz val="12"/>
-      <ma:u/>
-      <ma:scheme val="minor"/>
-    </ma:font>
-    <ma:font>
-      <ma:name val="宋体"/>
-      <ma:charset val="134"/>
-      <ma:family val="2"/>
-      <ma:color theme="11"/>
-      <ma:sz val="12"/>
-      <ma:u/>
-      <ma:scheme val="minor"/>
-    </ma:font>
-    <ma:font>
       <ma:name val="Hiragino Sans GB W3"/>
       <ma:charset val="134"/>
-      <ma:family val="3"/>
       <ma:sz val="14"/>
     </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FFFA7D00"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color theme="1"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="134"/>
+      <ma:b/>
+      <ma:color theme="3"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF0000FF"/>
+      <ma:sz val="11"/>
+      <ma:u/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color theme="0"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FFFF0000"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="134"/>
+      <ma:b/>
+      <ma:color theme="3"/>
+      <ma:sz val="18"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF800080"/>
+      <ma:sz val="11"/>
+      <ma:u/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:b/>
+      <ma:color rgb="FFFA7D00"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:b/>
+      <ma:color rgb="FFFFFFFF"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:i/>
+      <ma:color rgb="FF7F7F7F"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="134"/>
+      <ma:b/>
+      <ma:color theme="3"/>
+      <ma:sz val="15"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:b/>
+      <ma:color rgb="FF3F3F3F"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF006100"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF3F3F76"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="134"/>
+      <ma:b/>
+      <ma:color theme="3"/>
+      <ma:sz val="13"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF9C0006"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:color rgb="FF9C6500"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
+    <ma:font>
+      <ma:name val="宋体"/>
+      <ma:charset val="0"/>
+      <ma:b/>
+      <ma:color theme="1"/>
+      <ma:sz val="11"/>
+      <ma:scheme val="minor"/>
+    </ma:font>
   </ma:fonts>
-  <ma:fills count="3">
+  <ma:fills count="34">
     <ma:fill>
       <ma:patternFill patternType="none"/>
     </ma:fill>
@@ -133,8 +237,194 @@
         <ma:bgColor indexed="64"/>
       </ma:patternFill>
     </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="4" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="9" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="5"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="9" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="5" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFFFFFCC"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="6" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="4" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="9"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="5" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFF2F2F2"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFA5A5A5"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="4"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="8" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="5" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="6"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFC6EFCE"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFFFCC99"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="6" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="7" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="4" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="7"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="7" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="6" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFFFC7CE"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="9" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="FFFFEB9C"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="8" tint="0.399975585192419"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="8" tint="0.599993896298105"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="8"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor theme="7" tint="0.799981688894314"/>
+        <ma:bgColor indexed="64"/>
+      </ma:patternFill>
+    </ma:fill>
   </ma:fills>
-  <ma:borders count="2">
+  <ma:borders count="10">
     <ma:border>
       <ma:left/>
       <ma:right/>
@@ -157,45 +447,327 @@
       </ma:bottom>
       <ma:diagonal/>
     </ma:border>
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top/>
+      <ma:bottom style="double">
+        <ma:color rgb="FFFF8001"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top/>
+      <ma:bottom style="medium">
+        <ma:color theme="4" tint="0.499984740745262"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left style="thin">
+        <ma:color rgb="FFB2B2B2"/>
+      </ma:left>
+      <ma:right style="thin">
+        <ma:color rgb="FFB2B2B2"/>
+      </ma:right>
+      <ma:top style="thin">
+        <ma:color rgb="FFB2B2B2"/>
+      </ma:top>
+      <ma:bottom style="thin">
+        <ma:color rgb="FFB2B2B2"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left style="thin">
+        <ma:color rgb="FF7F7F7F"/>
+      </ma:left>
+      <ma:right style="thin">
+        <ma:color rgb="FF7F7F7F"/>
+      </ma:right>
+      <ma:top style="thin">
+        <ma:color rgb="FF7F7F7F"/>
+      </ma:top>
+      <ma:bottom style="thin">
+        <ma:color rgb="FF7F7F7F"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left style="double">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:left>
+      <ma:right style="double">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:right>
+      <ma:top style="double">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:top>
+      <ma:bottom style="double">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top/>
+      <ma:bottom style="medium">
+        <ma:color theme="4"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left style="thin">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:left>
+      <ma:right style="thin">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:right>
+      <ma:top style="thin">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:top>
+      <ma:bottom style="thin">
+        <ma:color rgb="FF3F3F3F"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top style="thin">
+        <ma:color theme="4"/>
+      </ma:top>
+      <ma:bottom style="double">
+        <ma:color theme="4"/>
+      </ma:bottom>
+      <ma:diagonal/>
+    </ma:border>
   </ma:borders>
-  <ma:cellStyleXfs count="3">
+  <ma:cellStyleXfs count="49">
     <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <ma:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <ma:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <ma:xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="15" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <ma:alignment vertical="center"/>
+    </ma:xf>
   </ma:cellStyleXfs>
   <ma:cellXfs count="7">
     <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <ma:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <ma:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <ma:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <ma:alignment horizontal="center"/>
-    </ma:xf>
-    <ma:xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <ma:alignment horizontal="center" vertical="center"/>
-    </ma:xf>
+    <ma:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <ma:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <ma:alignment horizontal="center" vertical="center"/>
     </ma:xf>
-    <ma:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <ma:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <ma:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <ma:alignment horizontal="center" vertical="center"/>
+    </ma:xf>
+    <ma:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <ma:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <ma:alignment horizontal="center"/>
+    </ma:xf>
   </ma:cellXfs>
-  <ma:cellStyles count="3">
+  <ma:cellStyles count="49">
     <ma:cellStyle name="常规" xfId="0" builtinId="0"/>
-    <ma:cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <ma:cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <ma:cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <ma:cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <ma:cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <ma:cellStyle name="输入" xfId="4" builtinId="20"/>
+    <ma:cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <ma:cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <ma:cellStyle name="货币" xfId="7" builtinId="4"/>
+    <ma:cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <ma:cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <ma:cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <ma:cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <ma:cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <ma:cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <ma:cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <ma:cellStyle name="计算" xfId="15" builtinId="22"/>
+    <ma:cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <ma:cellStyle name="适中" xfId="17" builtinId="28"/>
+    <ma:cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <ma:cellStyle name="好" xfId="19" builtinId="26"/>
+    <ma:cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <ma:cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <ma:cellStyle name="差" xfId="22" builtinId="27"/>
+    <ma:cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <ma:cellStyle name="输出" xfId="24" builtinId="21"/>
+    <ma:cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <ma:cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <ma:cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <ma:cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <ma:cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <ma:cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <ma:cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <ma:cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <ma:cellStyle name="标题" xfId="33" builtinId="15"/>
+    <ma:cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <ma:cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <ma:cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <ma:cellStyle name="注释" xfId="37" builtinId="10"/>
+    <ma:cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <ma:cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <ma:cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <ma:cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <ma:cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <ma:cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <ma:cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <ma:cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <ma:cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <ma:cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <ma:cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </ma:cellStyles>
-  <ma:dxfs count="0"/>
   <ma:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <ma:colors>
     <ma:mruColors>
-      <ma:color rgb="FFC8A6FF"/>
+      <ma:color rgb="00C8A6FF"/>
     </ma:mruColors>
   </ma:colors>
   <ma:extLst>
     <ma:ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <m:slicerStyles xmlns:m="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ma:ext>
-    <ma:ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <m:timelineStyles xmlns:m="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ma:ext>
   </ma:extLst>
 </ma:styleSheet>
@@ -517,133 +1089,130 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <ma:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <ma:dimension ref="A1:D4"/>
+  <ma:sheetPr/>
+  <ma:dimension ref="A1:E5"/>
   <ma:sheetViews>
     <ma:sheetView tabSelected="1" workbookViewId="0">
-      <ma:selection activeCell="B4" sqref="B4"/>
+      <ma:selection activeCell="D7" sqref="D7"/>
     </ma:sheetView>
   </ma:sheetViews>
-  <ma:sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
+  <ma:sheetFormatPr defaultColWidth="9" defaultRowHeight="20.4" outlineLevelRow="2" outlineLevelCol="4"/>
   <ma:cols>
-    <ma:col min="1" max="1" width="10.83203125" style="1"/>
-    <ma:col min="2" max="2" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <ma:col min="3" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <ma:col min="5" max="16384" width="10.83203125" style="1"/>
+    <ma:col min="1" max="1" width="9" style="1"/>
+    <ma:col min="2" max="2" width="11.1607142857143" style="1" customWidth="1"/>
+    <ma:col min="3" max="3" width="10.8303571428571" style="1"/>
+    <ma:col min="4" max="5" width="13.5" style="1" customWidth="1"/>
+    <ma:col min="6" max="16384" width="10.8303571428571" style="1"/>
   </ma:cols>
   <ma:sheetData>
-    <ma:row r="1" spans="1:4">
-      <ma:c r="A1" s="6" t="s">
+    <ma:row r="2" spans="2:5">
+      <ma:c r="A2"/>
+      <ma:c r="B2" s="2" t="s">
+        <ma:v>0</ma:v>
+      </ma:c>
+      <ma:c r="C2" s="3" t="s">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="D2" s="4" t="s">
+        <ma:v>2</ma:v>
+      </ma:c>
+      <ma:c r="E2" s="4" t="s">
         <ma:v>3</ma:v>
       </ma:c>
-      <ma:c r="B1" s="4" t="s">
-        <ma:v>0</ma:v>
-      </ma:c>
-      <ma:c r="C1" s="5" t="s">
-        <ma:v>1</ma:v>
-      </ma:c>
-      <ma:c r="D1" s="5" t="s">
-        <ma:v>2</ma:v>
-      </ma:c>
     </ma:row>
-    <ma:row r="2" spans="1:4">
-      <ma:c r="A2" s="2" t="s">
-        <ma:v>8</ma:v>
-      </ma:c>
-      <ma:c r="B2" s="2" t="n">
+    <ma:row r="3" spans="2:5">
+      <ma:c r="A3"/>
+      <ma:c r="B3" s="5" t="n">
         <ma:v>100</ma:v>
       </ma:c>
-      <ma:c r="C2" s="3" t="n">
+      <ma:c r="C3" s="5" t="s">
+        <ma:v>7</ma:v>
+      </ma:c>
+      <ma:c r="D3" s="6" t="n">
         <ma:v>50</ma:v>
       </ma:c>
-      <ma:c r="D2" s="2" t="n">
+      <ma:c r="E3" s="5" t="n">
         <ma:v>50</ma:v>
-      </ma:c>
-    </ma:row>
-    <ma:row r="3">
-      <ma:c r="A3" s="2" t="s">
-        <ma:v>9</ma:v>
-      </ma:c>
-      <ma:c r="B3" s="2" t="n">
-        <ma:v>200</ma:v>
-      </ma:c>
-      <ma:c r="C3" s="3" t="n">
-        <ma:v>60</ma:v>
-      </ma:c>
-      <ma:c r="D3" s="2" t="n">
-        <ma:v>140</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="4">
-      <ma:c r="A4" s="2" t="s">
-        <ma:v>10</ma:v>
-      </ma:c>
-      <ma:c r="B4" s="2" t="n">
+      <ma:c r="A4"/>
+      <ma:c r="B4" s="5" t="n">
+        <ma:v>200</ma:v>
+      </ma:c>
+      <ma:c r="C4" s="5" t="s">
+        <ma:v>8</ma:v>
+      </ma:c>
+      <ma:c r="D4" s="6" t="n">
+        <ma:v>60</ma:v>
+      </ma:c>
+      <ma:c r="E4" s="5" t="n">
+        <ma:v>140</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="5">
+      <ma:c r="A5"/>
+      <ma:c r="B5" s="5" t="n">
         <ma:v>300</ma:v>
       </ma:c>
-      <ma:c r="C4" s="3" t="n">
+      <ma:c r="C5" s="5" t="s">
+        <ma:v>9</ma:v>
+      </ma:c>
+      <ma:c r="D5" s="6" t="n">
         <ma:v>70</ma:v>
       </ma:c>
-      <ma:c r="D4" s="2" t="n">
+      <ma:c r="E5" s="5" t="n">
         <ma:v>240</ma:v>
       </ma:c>
     </ma:row>
   </ma:sheetData>
-  <ma:phoneticPr fontId="1" type="noConversion"/>
-  <ma:dataValidations count="1">
-    <ma:dataValidation type="list" operator="equal" showErrorMessage="1" sqref="A2:A5">
+  <ma:dataValidations count="2">
+    <ma:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <ma:formula1>Validation!$A$1:$A$3</ma:formula1>
+    </ma:dataValidation>
+    <ma:dataValidation type="list" operator="equal" showErrorMessage="1" sqref="C3:C6">
       <ma:formula1>'Validation'!$A$1:$A$3</ma:formula1>
       <ma:formula2>0</ma:formula2>
     </ma:dataValidation>
   </ma:dataValidations>
   <ma:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ma:extLst>
-    <ma:ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <m:dataValidations xmlns:m="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:r="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:ma="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <m:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" r:uid="{5205BA8A-4D43-4D41-9DB3-30DE2A9FCAA5}">
-          <m:formula1>
-            <ma:f>Validation!$A$1:$A$3</ma:f>
-          </m:formula1>
-          <ma:sqref>A2</ma:sqref>
-        </m:dataValidation>
-      </m:dataValidations>
-    </ma:ext>
-  </ma:extLst>
+  <ma:headerFooter/>
 </ma:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <ma:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:sheetPr/>
   <ma:dimension ref="A1:A3"/>
   <ma:sheetViews>
     <ma:sheetView workbookViewId="0">
       <ma:selection activeCell="A8" sqref="A8"/>
     </ma:sheetView>
   </ma:sheetViews>
-  <ma:sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <ma:sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelRow="2"/>
   <ma:sheetData>
     <ma:row r="1" spans="1:1">
       <ma:c r="A1" t="s">
-        <ma:v>5</ma:v>
+        <ma:v>4</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="2" spans="1:1">
       <ma:c r="A2" t="s">
-        <ma:v>6</ma:v>
+        <ma:v>5</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="3" spans="1:1">
       <ma:c r="A3" t="s">
-        <ma:v>7</ma:v>
+        <ma:v>6</ma:v>
       </ma:c>
     </ma:row>
   </ma:sheetData>
-  <ma:phoneticPr fontId="1" type="noConversion"/>
-  <ma:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ma:pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ma:headerFooter/>
 </ma:worksheet>
 </file>
</xml_diff>